<commit_message>
Added finance and criterion score in result pages.
</commit_message>
<xml_diff>
--- a/data/Sopra.xlsx
+++ b/data/Sopra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7410" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7410" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20 02 2017" sheetId="3" r:id="rId1"/>
@@ -943,7 +943,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -985,7 +985,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="7">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.17810000000000004</v>
+        <v>0.26310000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1037,11 +1037,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.26</v>
+        <v>0.24</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4200000000000003E-2</v>
+        <v>4.0800000000000003E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1392,7 +1392,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="7">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.1197</v>
+        <v>-8.77E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1444,11 +1444,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.27</v>
+        <v>-0.95</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5900000000000003E-2</v>
+        <v>-0.1615</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1799,7 +1799,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.11070000000000003</v>
+        <v>3.2500000000000029E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1851,11 +1851,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.18</v>
+        <v>-0.64</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0600000000000002E-2</v>
+        <v>-0.10880000000000001</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2209,7 +2209,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="21">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.22720000000000001</v>
+        <v>0.24420000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2261,11 +2261,11 @@
       </c>
       <c r="C5" s="21">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.77</v>
+        <v>0.87</v>
       </c>
       <c r="D5" s="21">
         <f ca="1">B5*C5</f>
-        <v>0.13090000000000002</v>
+        <v>0.1479</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -2619,7 +2619,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="21">
         <f ca="1">SUM(D2:D5)</f>
-        <v>7.010000000000001E-2</v>
+        <v>-0.1492</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,11 +2671,11 @@
       </c>
       <c r="C5" s="21">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.64</v>
+        <v>-0.65</v>
       </c>
       <c r="D5" s="21">
         <f ca="1">B5*C5</f>
-        <v>0.10880000000000001</v>
+        <v>-0.11050000000000001</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -2983,8 +2983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3029,7 +3029,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="21">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.16720000000000002</v>
+        <v>-6.9100000000000009E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3081,11 +3081,11 @@
       </c>
       <c r="C5" s="21">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.47</v>
+        <v>-0.92</v>
       </c>
       <c r="D5" s="21">
         <f ca="1">B5*C5</f>
-        <v>7.9899999999999999E-2</v>
+        <v>-0.15640000000000001</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>

</xml_diff>

<commit_message>
Updated all scores for 16/03/2017
</commit_message>
<xml_diff>
--- a/data/Sopra.xlsx
+++ b/data/Sopra.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Python\StockChooser\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.smith.15\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="24 02 2017" sheetId="5" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="13 03 2017" sheetId="16" r:id="rId12"/>
     <sheet name="14 03 2017" sheetId="17" r:id="rId13"/>
     <sheet name="15 03 2017" sheetId="18" r:id="rId14"/>
+    <sheet name="16 03 2017" sheetId="19" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="95">
   <si>
     <t>Critère</t>
   </si>
@@ -326,12 +327,30 @@
   <si>
     <t>le RSI reste proche de la ligne 50</t>
   </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>le MACD reste au dessus du signal</t>
+  </si>
+  <si>
+    <t>Le RSI depasse la ligne 70</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k est au dessus des autres courbes </t>
+  </si>
+  <si>
+    <t>0,7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -557,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1717,14 +1736,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1761,10 +1780,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>-0.14750000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-0.13730000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -1785,7 +1804,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -1804,7 +1823,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -1813,17 +1832,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.64</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>-0.10880000000000001</v>
+        <v>-9.8600000000000007E-2</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1832,7 +1851,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1841,7 +1860,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1850,7 +1869,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1859,7 +1878,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -1878,7 +1897,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1917,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -1918,7 +1937,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -1938,7 +1957,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -1958,7 +1977,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -1978,7 +1997,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -1987,7 +2006,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1996,7 +2015,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -2005,7 +2024,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -2024,7 +2043,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -2042,7 +2061,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -2060,7 +2079,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -2078,7 +2097,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -2096,7 +2115,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -2132,12 +2151,12 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="10.85546875" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2177,7 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2176,12 +2195,12 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.11219999999999999</v>
+        <v>4.5899999999999989E-2</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -2204,7 +2223,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2225,7 +2244,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -2234,11 +2253,11 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.12</v>
+        <v>-0.27</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">B5*C5</f>
-        <v>2.0400000000000001E-2</v>
+        <v>-4.5900000000000003E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2246,7 +2265,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2257,7 +2276,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2268,7 +2287,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2279,7 +2298,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2290,7 +2309,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2311,7 +2330,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2333,7 +2352,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -2355,7 +2374,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -2377,7 +2396,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -2399,7 +2418,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -2421,7 +2440,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="11"/>
@@ -2432,7 +2451,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2443,7 +2462,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2454,7 +2473,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2475,7 +2494,7 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2495,7 +2514,7 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -2515,7 +2534,7 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -2535,7 +2554,7 @@
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -2555,7 +2574,7 @@
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -2593,12 +2612,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="10.85546875" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2619,7 +2638,7 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2637,12 +2656,12 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.19770000000000001</v>
+        <v>0.40340000000000004</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -2665,7 +2684,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2686,7 +2705,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -2695,11 +2714,11 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.33</v>
+        <v>0.88</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">B5*C5</f>
-        <v>-5.6100000000000004E-2</v>
+        <v>0.14960000000000001</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2707,7 +2726,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2718,7 +2737,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2729,7 +2748,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2740,7 +2759,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2751,7 +2770,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2772,7 +2791,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2794,7 +2813,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -2816,7 +2835,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -2838,7 +2857,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -2860,7 +2879,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -2882,7 +2901,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="11"/>
@@ -2893,7 +2912,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2904,7 +2923,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2915,7 +2934,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2936,7 +2955,7 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2956,7 +2975,7 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -2976,7 +2995,7 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -2996,7 +3015,7 @@
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -3016,7 +3035,7 @@
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -3054,12 +3073,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="10.85546875" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3080,7 +3099,7 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3098,12 +3117,12 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9">
         <f ca="1">SUM(D2:D5)</f>
-        <v>7.9000000000000015E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3126,7 +3145,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -3147,7 +3166,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -3156,11 +3175,11 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.56000000000000005</v>
+        <v>0.36</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">B5*C5</f>
-        <v>9.5200000000000021E-2</v>
+        <v>6.1200000000000004E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3168,7 +3187,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3179,7 +3198,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3190,7 +3209,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3201,7 +3220,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3212,7 +3231,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3233,7 +3252,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3255,7 +3274,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -3277,7 +3296,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -3299,7 +3318,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -3321,7 +3340,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -3343,7 +3362,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="11"/>
@@ -3354,7 +3373,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3365,7 +3384,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3376,7 +3395,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3397,7 +3416,7 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -3417,7 +3436,7 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -3437,7 +3456,7 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -3457,7 +3476,7 @@
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -3477,7 +3496,7 @@
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -3515,12 +3534,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="10.85546875" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3541,7 +3560,7 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3559,12 +3578,12 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9">
         <f ca="1">SUM(D2:D5)</f>
-        <v>5.4800000000000001E-2</v>
+        <v>0.12620000000000001</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3587,7 +3606,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -3608,7 +3627,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -3617,11 +3636,11 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.35</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">B5*C5</f>
-        <v>-5.9499999999999997E-2</v>
+        <v>1.1900000000000003E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3629,7 +3648,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3640,7 +3659,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3651,7 +3670,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3662,7 +3681,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3673,7 +3692,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3694,7 +3713,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3716,7 +3735,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -3738,7 +3757,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -3760,7 +3779,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -3782,7 +3801,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -3804,7 +3823,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="11"/>
@@ -3815,7 +3834,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3826,7 +3845,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3837,7 +3856,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3858,7 +3877,7 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -3878,7 +3897,7 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -3898,7 +3917,7 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -3918,7 +3937,7 @@
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -3938,7 +3957,7 @@
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -3973,15 +3992,15 @@
   <dimension ref="A1:IV24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="10.85546875" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -4002,7 +4021,7 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -4020,12 +4039,12 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.1153</v>
+        <v>0.1527</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -4048,7 +4067,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -4069,7 +4088,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -4078,11 +4097,11 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.1</v>
+        <v>0.12</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">B5*C5</f>
-        <v>-1.7000000000000001E-2</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -4090,7 +4109,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -4101,7 +4120,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -4112,7 +4131,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4123,7 +4142,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4134,7 +4153,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4155,7 +4174,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -4177,7 +4196,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -4199,7 +4218,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -4221,7 +4240,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -4243,7 +4262,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -4265,7 +4284,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="11"/>
@@ -4276,7 +4295,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4287,7 +4306,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4298,7 +4317,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -4319,7 +4338,7 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -4339,7 +4358,7 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -4359,7 +4378,7 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -4379,7 +4398,7 @@
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -4399,7 +4418,7 @@
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -4429,18 +4448,471 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <f>B2*C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="9">
+        <f ca="1">SUM(D2:D5)</f>
+        <v>0.24510000000000004</v>
+      </c>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" ht="15">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C3" s="10">
+        <f>SUM(D11:D15)</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="D3" s="9">
+        <f>B3*C3</f>
+        <v>0.13050000000000003</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" ht="15">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C4" s="9">
+        <f>SUM(D20:D24)</f>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="D4" s="9">
+        <f>B4*C4</f>
+        <v>7.3800000000000004E-2</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="1:9" ht="15">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="C5" s="9">
+        <f ca="1">RANDBETWEEN(-100,100)/100</f>
+        <v>0.24</v>
+      </c>
+      <c r="D5" s="9">
+        <f ca="1">B5*C5</f>
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="1:9" ht="15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+    </row>
+    <row r="7" spans="1:9" ht="15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" ht="15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="1:9" ht="15">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+    </row>
+    <row r="11" spans="1:9" ht="15">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="40">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <f>B11*C13</f>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+    </row>
+    <row r="12" spans="1:9" ht="15">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="8">
+        <f>B12*C12</f>
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="8">
+        <f>B13*C13</f>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+    </row>
+    <row r="14" spans="1:9" ht="15">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="8">
+        <f>B14*C14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+    </row>
+    <row r="15" spans="1:9" ht="15">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <f>B15*C15</f>
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+    </row>
+    <row r="16" spans="1:9" ht="15">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+    </row>
+    <row r="17" spans="1:9" ht="15">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="1:9" ht="15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="1:9" ht="15">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+    </row>
+    <row r="20" spans="1:9" ht="15">
+      <c r="A20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="D20" s="9">
+        <f>B20*C20</f>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C21" s="9">
+        <v>-0.44</v>
+      </c>
+      <c r="D21" s="9">
+        <f>B21*C21</f>
+        <v>-8.8000000000000009E-2</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+    </row>
+    <row r="22" spans="1:9" ht="15">
+      <c r="A22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="D22" s="9">
+        <f>B22*C22</f>
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+    </row>
+    <row r="23" spans="1:9" ht="15">
+      <c r="A23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.44</v>
+      </c>
+      <c r="D23" s="8">
+        <f>B23*C23</f>
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+    </row>
+    <row r="24" spans="1:9" ht="15">
+      <c r="A24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="D24" s="8">
+        <f>B24*C24</f>
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -4459,7 +4931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -4477,10 +4949,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.32110000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.52850000000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -4501,7 +4973,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -4520,7 +4992,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -4529,17 +5001,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.86</v>
+        <v>0.36</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>-0.1462</v>
+        <v>6.1200000000000004E-2</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -4548,7 +5020,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -4557,7 +5029,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4566,7 +5038,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -4575,7 +5047,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -4594,7 +5066,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -4614,7 +5086,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -4634,7 +5106,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -4654,7 +5126,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -4674,7 +5146,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -4694,7 +5166,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -4703,7 +5175,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -4712,7 +5184,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -4721,7 +5193,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -4740,7 +5212,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -4758,7 +5230,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -4776,7 +5248,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -4794,7 +5266,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -4812,7 +5284,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -4846,12 +5318,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -4870,7 +5342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -4888,10 +5360,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.25690000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.25010000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -4912,7 +5384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -4931,7 +5403,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -4940,17 +5412,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>0.11560000000000002</v>
+        <v>0.10880000000000001</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -4959,7 +5431,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -4968,7 +5440,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4977,7 +5449,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -4986,7 +5458,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -5005,7 +5477,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -5025,7 +5497,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -5045,7 +5517,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -5065,7 +5537,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -5085,7 +5557,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -5105,7 +5577,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -5114,7 +5586,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -5123,7 +5595,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -5132,7 +5604,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -5151,7 +5623,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -5169,7 +5641,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -5187,7 +5659,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -5205,7 +5677,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -5223,7 +5695,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -5257,12 +5729,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -5281,7 +5753,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -5299,10 +5771,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.21560000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6.5000000000000058E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -5323,7 +5795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -5342,7 +5814,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -5351,17 +5823,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.49</v>
+        <v>-0.74</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>8.3299999999999999E-2</v>
+        <v>-0.1258</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -5370,7 +5842,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -5379,7 +5851,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5388,7 +5860,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -5397,7 +5869,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -5416,7 +5888,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -5436,7 +5908,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -5456,7 +5928,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -5476,7 +5948,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -5496,7 +5968,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -5516,7 +5988,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -5525,7 +5997,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -5534,7 +6006,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -5543,7 +6015,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -5562,7 +6034,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -5580,7 +6052,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -5598,7 +6070,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -5616,7 +6088,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -5634,7 +6106,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -5668,12 +6140,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -5692,7 +6164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -5710,10 +6182,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.33310000000000006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5.6000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -5734,7 +6206,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -5753,7 +6225,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -5762,17 +6234,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.89</v>
+        <v>-0.74</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>0.15130000000000002</v>
+        <v>-0.1258</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -5781,7 +6253,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -5790,7 +6262,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5799,7 +6271,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -5808,7 +6280,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -5827,7 +6299,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -5847,7 +6319,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -5867,7 +6339,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -5887,7 +6359,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -5907,7 +6379,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -5927,7 +6399,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -5936,7 +6408,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -5945,7 +6417,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -5954,7 +6426,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -5973,7 +6445,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -5991,7 +6463,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -6009,7 +6481,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -6027,7 +6499,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -6045,7 +6517,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -6079,12 +6551,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6103,7 +6575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -6121,10 +6593,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.13520000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.18620000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -6145,7 +6617,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -6164,7 +6636,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -6173,17 +6645,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.38</v>
+        <v>-0.08</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>-6.4600000000000005E-2</v>
+        <v>-1.3600000000000001E-2</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -6192,7 +6664,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -6201,7 +6673,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6210,7 +6682,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -6219,7 +6691,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -6238,7 +6710,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -6258,7 +6730,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -6278,7 +6750,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -6298,7 +6770,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -6318,7 +6790,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -6338,7 +6810,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -6347,7 +6819,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -6356,7 +6828,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -6365,7 +6837,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -6384,7 +6856,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -6402,7 +6874,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -6420,7 +6892,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -6438,7 +6910,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -6456,7 +6928,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -6490,12 +6962,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6514,7 +6986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -6532,10 +7004,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.16500000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.15650000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -6556,7 +7028,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -6575,7 +7047,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -6584,17 +7056,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>1.0200000000000001E-2</v>
+        <v>1.7000000000000001E-3</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -6603,7 +7075,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -6612,7 +7084,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6621,7 +7093,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -6630,7 +7102,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -6649,7 +7121,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -6669,7 +7141,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -6689,7 +7161,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -6709,7 +7181,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -6729,7 +7201,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -6749,7 +7221,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -6758,7 +7230,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -6767,7 +7239,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -6776,7 +7248,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -6795,7 +7267,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -6813,7 +7285,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -6831,7 +7303,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -6849,7 +7321,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -6867,7 +7339,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -6901,12 +7373,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6925,7 +7397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -6943,10 +7415,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.25440000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.15240000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -6967,7 +7439,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -6986,7 +7458,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -6995,17 +7467,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>0.93</v>
+        <v>0.33</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>0.15810000000000002</v>
+        <v>5.6100000000000004E-2</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -7014,7 +7486,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -7023,7 +7495,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -7032,7 +7504,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -7041,7 +7513,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -7060,7 +7532,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -7080,7 +7552,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -7100,7 +7572,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -7120,7 +7592,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -7140,7 +7612,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -7160,7 +7632,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -7169,7 +7641,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -7178,7 +7650,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -7187,7 +7659,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -7206,7 +7678,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -7224,7 +7696,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -7242,7 +7714,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -7260,7 +7732,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -7278,7 +7750,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
@@ -7312,12 +7784,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="256" width="14.42578125" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -7336,7 +7808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -7354,10 +7826,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="22">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.10569999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5.8099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -7378,7 +7850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -7397,7 +7869,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
@@ -7406,17 +7878,17 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">RANDBETWEEN(-100,100)/100</f>
-        <v>-0.13</v>
+        <v>-0.41</v>
       </c>
       <c r="D5" s="22">
         <f ca="1">B5*C5</f>
-        <v>-2.2100000000000002E-2</v>
+        <v>-6.9699999999999998E-2</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -7425,7 +7897,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -7434,7 +7906,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -7443,7 +7915,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -7452,7 +7924,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -7471,7 +7943,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -7491,7 +7963,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -7511,7 +7983,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -7531,7 +8003,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -7551,7 +8023,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
@@ -7571,7 +8043,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="24"/>
@@ -7580,7 +8052,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -7589,7 +8061,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -7598,7 +8070,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
@@ -7617,7 +8089,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
@@ -7635,7 +8107,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
@@ -7653,7 +8125,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
@@ -7671,7 +8143,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -7689,7 +8161,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>23</v>
       </c>

</xml_diff>